<commit_message>
Update controller layout spreadsheet
Added current plans for robot controls to the controller layout
spreadsheet in addition to relevant pictures of the controllers for
reference
</commit_message>
<xml_diff>
--- a/2016 Stronghold Summer Robot Controller Layout.xlsx
+++ b/2016 Stronghold Summer Robot Controller Layout.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcrc\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="X-Box Controller" sheetId="1" r:id="rId1"/>
     <sheet name="Joysticks" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>X-Box Controller</t>
   </si>
@@ -57,50 +52,89 @@
     <t>Left</t>
   </si>
   <si>
-    <t>Left 90 Degree Turn</t>
-  </si>
-  <si>
     <t>Right</t>
   </si>
   <si>
-    <t>Right 90 Degree Turn</t>
-  </si>
-  <si>
     <t>Down</t>
   </si>
   <si>
-    <t>180 Degree Turn</t>
-  </si>
-  <si>
     <t>Buttons</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>Arm Down</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Arm Up</t>
-  </si>
-  <si>
     <t>Arcade Drive</t>
   </si>
   <si>
     <t>Right Trigger</t>
   </si>
   <si>
-    <t>Fine Drive Control</t>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Arm Up?</t>
+  </si>
+  <si>
+    <t>Arm Down?</t>
+  </si>
+  <si>
+    <t>Fine Drive Control?</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Left Trigger</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Bumpers</t>
+  </si>
+  <si>
+    <t>Left Bumper</t>
+  </si>
+  <si>
+    <t>Right Bumper</t>
+  </si>
+  <si>
+    <t>Joystick 1</t>
+  </si>
+  <si>
+    <t>Joystick 2</t>
+  </si>
+  <si>
+    <t>Joystick</t>
+  </si>
+  <si>
+    <t>Axes</t>
+  </si>
+  <si>
+    <t>Throttle</t>
+  </si>
+  <si>
+    <t>Left Joystick Button</t>
+  </si>
+  <si>
+    <t>Right Joystick Button</t>
+  </si>
+  <si>
+    <t>Select/Back</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +163,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -152,6 +189,331 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="71J8QzMGahL._SL1300_.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="5334000"/>
+          <a:ext cx="12382500" cy="12382500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>416700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>35700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>169050</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>159525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="1638b1b81183871c981f49b04c4c0966.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5255400" y="2321700"/>
+          <a:ext cx="5238750" cy="2600325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>345300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>243700</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Logitech Attack 3 Left View.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9365475" y="5610225"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>92850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>102375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Logitech Attack 3 Right View.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180975" y="5807850"/>
+          <a:ext cx="8858250" cy="12392025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9344025" y="6324600"/>
+          <a:ext cx="352425" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7143750" y="6448425"/>
+          <a:ext cx="2200275" cy="1695450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9696450" y="6448425"/>
+          <a:ext cx="4314825" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -197,7 +559,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,7 +594,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,34 +771,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -444,12 +806,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -457,10 +819,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -468,80 +830,117 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -549,19 +948,167 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix manual override motor safety issue and update controller layout spreadsheet
Fixed a safety issue with manual overrides (motors were not set to zero
when manual overriding was disabled) and updated the controller layout
spreadsheet to match currently known controls
</commit_message>
<xml_diff>
--- a/2016 Stronghold Summer Robot Controller Layout.xlsx
+++ b/2016 Stronghold Summer Robot Controller Layout.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\2016-stronghold-summer-robot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="X-Box Controller" sheetId="1" r:id="rId1"/>
     <sheet name="Joysticks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>X-Box Controller</t>
   </si>
@@ -76,12 +81,6 @@
     <t>Up</t>
   </si>
   <si>
-    <t>Arm Up?</t>
-  </si>
-  <si>
-    <t>Arm Down?</t>
-  </si>
-  <si>
     <t>Fine Drive Control?</t>
   </si>
   <si>
@@ -128,13 +127,25 @@
   </si>
   <si>
     <t>Select/Back</t>
+  </si>
+  <si>
+    <t>Ball Intake</t>
+  </si>
+  <si>
+    <t>Fire Ball Shooter</t>
+  </si>
+  <si>
+    <t>Arm Up</t>
+  </si>
+  <si>
+    <t>Arm Down</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,34 +782,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -806,12 +817,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -822,7 +833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -830,117 +841,129 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -953,23 +976,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
@@ -977,7 +1000,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -987,28 +1010,28 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1020,84 +1043,95 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2"/>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
+      <c r="C10" t="s">
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Revise ball shooter tasks and overrides to reflect current robot design, build VI from vision script, and update layout spreadsheet
Revised ball shooter tasks (added VIs "Set Weave Lift Motor Output.vi",
"Move Arm to Limit Switch.vi", and "Move Weave to Limit Switch.vi") and
manual overrides in "Periodic Tasks.vi" to reflect current robot design
and built VI from the vision processing script (includes feedback value
calculation); updated controller layout spreadsheet
</commit_message>
<xml_diff>
--- a/2016 Stronghold Summer Robot Controller Layout.xlsx
+++ b/2016 Stronghold Summer Robot Controller Layout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240"/>
   </bookViews>
   <sheets>
     <sheet name="X-Box Controller" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>X-Box Controller</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>Arm Down</t>
+  </si>
+  <si>
+    <t>Winch Down</t>
+  </si>
+  <si>
+    <t>Winch Up</t>
+  </si>
+  <si>
+    <t>Weave Lift Down</t>
+  </si>
+  <si>
+    <t>Weave Lift Up</t>
   </si>
 </sst>
 </file>
@@ -792,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -875,11 +887,23 @@
       <c r="A12" t="s">
         <v>17</v>
       </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -910,12 +934,24 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -979,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1092,11 +1128,23 @@
       <c r="A11">
         <v>4</v>
       </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1126,14 +1174,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more dashboard data and fix issue in "Drive Tasks.vi"
Add more dashboard data (a new Graphs tab with motor graphs in place of
the unused Basic tab and limit switch and IR Breakbeam indicators) and
fixed an issue that could cause early termination of the aiming
procedure
</commit_message>
<xml_diff>
--- a/2016 Stronghold Summer Robot Controller Layout.xlsx
+++ b/2016 Stronghold Summer Robot Controller Layout.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\2016-stronghold-summer-robot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="X-Box Controller" sheetId="1" r:id="rId1"/>
     <sheet name="Joysticks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
   <si>
     <t>X-Box Controller</t>
   </si>
@@ -96,9 +91,6 @@
     <t>Start</t>
   </si>
   <si>
-    <t>Bumpers</t>
-  </si>
-  <si>
     <t>Left Bumper</t>
   </si>
   <si>
@@ -151,13 +143,19 @@
   </si>
   <si>
     <t>Weave Lift Up</t>
+  </si>
+  <si>
+    <t>Ball Aim</t>
+  </si>
+  <si>
+    <t>Triggers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,6 +194,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,34 +798,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:3">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -829,12 +833,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -845,7 +849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -853,137 +857,143 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
       <c r="C19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
@@ -992,14 +1002,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1012,62 +1022,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:5">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1079,121 +1089,126 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>